<commit_message>
Atualizada planilha de calibração do pêndulo
</commit_message>
<xml_diff>
--- a/Resources/Calibração pendulo.xlsx
+++ b/Resources/Calibração pendulo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14240" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>V1</t>
   </si>
@@ -40,12 +40,6 @@
   </si>
   <si>
     <t>d</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>T</t>
   </si>
   <si>
     <t>regua</t>
@@ -387,7 +381,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -693,10 +687,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -744,85 +738,35 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B6">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B7">
-        <v>0.98</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="E7" t="s">
+      <c r="C6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B8">
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="E8" t="s">
+      <c r="C8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B9">
-        <v>1.03</v>
-      </c>
-    </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B10">
-        <v>1.06</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="B10" t="s">
         <v>11</v>
       </c>
-      <c r="E10" t="s">
+      <c r="C10" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B12">
-        <v>1.05</v>
-      </c>
-      <c r="D12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B13">
-        <v>1.03</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B14">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B15">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualizada a planilha com curvas de calibração do pendulo
</commit_message>
<xml_diff>
--- a/Resources/Calibração pendulo.xlsx
+++ b/Resources/Calibração pendulo.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14240" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>V1</t>
   </si>
@@ -382,7 +383,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection sqref="A1:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -689,7 +690,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -772,4 +773,312 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>2.91</v>
+      </c>
+      <c r="C2">
+        <v>2.78</v>
+      </c>
+      <c r="E2" t="str">
+        <f>CONCATENATE("{",A2,",",B2,",",C2,"},")</f>
+        <v>{0,2.91,2.78},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="C3">
+        <v>2.44</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E20" si="0">CONCATENATE("{",A3,",",B3,",",C3,"},")</f>
+        <v>{10,2.51,2.44},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>2.16</v>
+      </c>
+      <c r="C4">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>{20,2.16,2.18},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>30</v>
+      </c>
+      <c r="B5">
+        <v>1.82</v>
+      </c>
+      <c r="C5">
+        <v>1.7</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v>{30,1.82,1.7},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>40</v>
+      </c>
+      <c r="B6">
+        <v>1.47</v>
+      </c>
+      <c r="C6">
+        <v>1.39</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="0"/>
+        <v>{40,1.47,1.39},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>50</v>
+      </c>
+      <c r="B7">
+        <v>1.21</v>
+      </c>
+      <c r="C7">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="0"/>
+        <v>{50,1.21,1.12},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>60</v>
+      </c>
+      <c r="B8">
+        <v>0.86</v>
+      </c>
+      <c r="C8">
+        <v>0.85</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="0"/>
+        <v>{60,0.86,0.85},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>70</v>
+      </c>
+      <c r="B9">
+        <v>0.622</v>
+      </c>
+      <c r="C9">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="0"/>
+        <v>{70,0.622,0.582},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>80</v>
+      </c>
+      <c r="B10">
+        <v>0.37</v>
+      </c>
+      <c r="C10">
+        <v>0.32</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="0"/>
+        <v>{80,0.37,0.32},</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>90</v>
+      </c>
+      <c r="B11">
+        <v>0.5</v>
+      </c>
+      <c r="C11">
+        <v>0.7</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="0"/>
+        <v>{90,0.5,0.7},</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>100</v>
+      </c>
+      <c r="B12">
+        <v>0.24</v>
+      </c>
+      <c r="C12">
+        <v>0.25</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="0"/>
+        <v>{100,0.24,0.25},</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>110</v>
+      </c>
+      <c r="B13">
+        <v>-0.54</v>
+      </c>
+      <c r="C13">
+        <v>-0.56999999999999995</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="0"/>
+        <v>{110,-0.54,-0.57},</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>120</v>
+      </c>
+      <c r="B14">
+        <v>-0.82</v>
+      </c>
+      <c r="C14">
+        <v>-0.81</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="0"/>
+        <v>{120,-0.82,-0.81},</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>130</v>
+      </c>
+      <c r="B15">
+        <v>-1.05</v>
+      </c>
+      <c r="C15">
+        <v>-1.06</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="0"/>
+        <v>{130,-1.05,-1.06},</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>140</v>
+      </c>
+      <c r="B16">
+        <v>-1.34</v>
+      </c>
+      <c r="C16">
+        <v>-1.37</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="0"/>
+        <v>{140,-1.34,-1.37},</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>150</v>
+      </c>
+      <c r="B17">
+        <v>-1.58</v>
+      </c>
+      <c r="C17">
+        <v>-1.57</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="0"/>
+        <v>{150,-1.58,-1.57},</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>160</v>
+      </c>
+      <c r="B18">
+        <v>-1.98</v>
+      </c>
+      <c r="C18">
+        <v>-1.89</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="0"/>
+        <v>{160,-1.98,-1.89},</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>170</v>
+      </c>
+      <c r="B19">
+        <v>-2.27</v>
+      </c>
+      <c r="C19">
+        <v>-2.21</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="0"/>
+        <v>{170,-2.27,-2.21},</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>180</v>
+      </c>
+      <c r="B20">
+        <v>-2.61</v>
+      </c>
+      <c r="C20" s="1">
+        <v>-2.57</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="0"/>
+        <v>{180,-2.61,-2.57},</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Melhorada a apresentação dos resultados do pêndulo
</commit_message>
<xml_diff>
--- a/Resources/Calibração pendulo.xlsx
+++ b/Resources/Calibração pendulo.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14240" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sem condicionamento" sheetId="1" r:id="rId1"/>
+    <sheet name="Com condicionamento" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -383,7 +383,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E20"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -687,6 +687,314 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>2.91</v>
+      </c>
+      <c r="C2">
+        <v>2.78</v>
+      </c>
+      <c r="E2" t="str">
+        <f>CONCATENATE("{",ABS(A2-180),",",B2,",",C2,"},")</f>
+        <v>{180,2.91,2.78},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="C3">
+        <v>2.44</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E20" si="0">CONCATENATE("{",ABS(A3-180),",",B3,",",C3,"},")</f>
+        <v>{170,2.51,2.44},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>2.16</v>
+      </c>
+      <c r="C4">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>{160,2.16,2.18},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>30</v>
+      </c>
+      <c r="B5">
+        <v>1.82</v>
+      </c>
+      <c r="C5">
+        <v>1.7</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v>{150,1.82,1.7},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>40</v>
+      </c>
+      <c r="B6">
+        <v>1.47</v>
+      </c>
+      <c r="C6">
+        <v>1.39</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="0"/>
+        <v>{140,1.47,1.39},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>50</v>
+      </c>
+      <c r="B7">
+        <v>1.21</v>
+      </c>
+      <c r="C7">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="0"/>
+        <v>{130,1.21,1.12},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>60</v>
+      </c>
+      <c r="B8">
+        <v>0.86</v>
+      </c>
+      <c r="C8">
+        <v>0.85</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="0"/>
+        <v>{120,0.86,0.85},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>70</v>
+      </c>
+      <c r="B9">
+        <v>0.622</v>
+      </c>
+      <c r="C9">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="0"/>
+        <v>{110,0.622,0.582},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>80</v>
+      </c>
+      <c r="B10">
+        <v>0.37</v>
+      </c>
+      <c r="C10">
+        <v>0.32</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="0"/>
+        <v>{100,0.37,0.32},</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>90</v>
+      </c>
+      <c r="B11">
+        <v>0.5</v>
+      </c>
+      <c r="C11">
+        <v>0.7</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="0"/>
+        <v>{90,0.5,0.7},</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>100</v>
+      </c>
+      <c r="B12">
+        <v>0.24</v>
+      </c>
+      <c r="C12">
+        <v>0.25</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="0"/>
+        <v>{80,0.24,0.25},</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>110</v>
+      </c>
+      <c r="B13">
+        <v>-0.54</v>
+      </c>
+      <c r="C13">
+        <v>-0.56999999999999995</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="0"/>
+        <v>{70,-0.54,-0.57},</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>120</v>
+      </c>
+      <c r="B14">
+        <v>-0.82</v>
+      </c>
+      <c r="C14">
+        <v>-0.81</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="0"/>
+        <v>{60,-0.82,-0.81},</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>130</v>
+      </c>
+      <c r="B15">
+        <v>-1.05</v>
+      </c>
+      <c r="C15">
+        <v>-1.06</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="0"/>
+        <v>{50,-1.05,-1.06},</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>140</v>
+      </c>
+      <c r="B16">
+        <v>-1.34</v>
+      </c>
+      <c r="C16">
+        <v>-1.37</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="0"/>
+        <v>{40,-1.34,-1.37},</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>150</v>
+      </c>
+      <c r="B17">
+        <v>-1.58</v>
+      </c>
+      <c r="C17">
+        <v>-1.57</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="0"/>
+        <v>{30,-1.58,-1.57},</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>160</v>
+      </c>
+      <c r="B18">
+        <v>-1.98</v>
+      </c>
+      <c r="C18">
+        <v>-1.89</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="0"/>
+        <v>{20,-1.98,-1.89},</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>170</v>
+      </c>
+      <c r="B19">
+        <v>-2.27</v>
+      </c>
+      <c r="C19">
+        <v>-2.21</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="0"/>
+        <v>{10,-2.27,-2.21},</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>180</v>
+      </c>
+      <c r="B20">
+        <v>-2.61</v>
+      </c>
+      <c r="C20" s="1">
+        <v>-2.57</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="0"/>
+        <v>{0,-2.61,-2.57},</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
@@ -773,312 +1081,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>2.91</v>
-      </c>
-      <c r="C2">
-        <v>2.78</v>
-      </c>
-      <c r="E2" t="str">
-        <f>CONCATENATE("{",A2,",",B2,",",C2,"},")</f>
-        <v>{0,2.91,2.78},</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>10</v>
-      </c>
-      <c r="B3">
-        <v>2.5099999999999998</v>
-      </c>
-      <c r="C3">
-        <v>2.44</v>
-      </c>
-      <c r="E3" t="str">
-        <f t="shared" ref="E3:E20" si="0">CONCATENATE("{",A3,",",B3,",",C3,"},")</f>
-        <v>{10,2.51,2.44},</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>20</v>
-      </c>
-      <c r="B4">
-        <v>2.16</v>
-      </c>
-      <c r="C4">
-        <v>2.1800000000000002</v>
-      </c>
-      <c r="E4" t="str">
-        <f t="shared" si="0"/>
-        <v>{20,2.16,2.18},</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>30</v>
-      </c>
-      <c r="B5">
-        <v>1.82</v>
-      </c>
-      <c r="C5">
-        <v>1.7</v>
-      </c>
-      <c r="E5" t="str">
-        <f t="shared" si="0"/>
-        <v>{30,1.82,1.7},</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>40</v>
-      </c>
-      <c r="B6">
-        <v>1.47</v>
-      </c>
-      <c r="C6">
-        <v>1.39</v>
-      </c>
-      <c r="E6" t="str">
-        <f t="shared" si="0"/>
-        <v>{40,1.47,1.39},</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>50</v>
-      </c>
-      <c r="B7">
-        <v>1.21</v>
-      </c>
-      <c r="C7">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="E7" t="str">
-        <f t="shared" si="0"/>
-        <v>{50,1.21,1.12},</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>60</v>
-      </c>
-      <c r="B8">
-        <v>0.86</v>
-      </c>
-      <c r="C8">
-        <v>0.85</v>
-      </c>
-      <c r="E8" t="str">
-        <f t="shared" si="0"/>
-        <v>{60,0.86,0.85},</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>70</v>
-      </c>
-      <c r="B9">
-        <v>0.622</v>
-      </c>
-      <c r="C9">
-        <v>0.58199999999999996</v>
-      </c>
-      <c r="E9" t="str">
-        <f t="shared" si="0"/>
-        <v>{70,0.622,0.582},</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>80</v>
-      </c>
-      <c r="B10">
-        <v>0.37</v>
-      </c>
-      <c r="C10">
-        <v>0.32</v>
-      </c>
-      <c r="E10" t="str">
-        <f t="shared" si="0"/>
-        <v>{80,0.37,0.32},</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>90</v>
-      </c>
-      <c r="B11">
-        <v>0.5</v>
-      </c>
-      <c r="C11">
-        <v>0.7</v>
-      </c>
-      <c r="E11" t="str">
-        <f t="shared" si="0"/>
-        <v>{90,0.5,0.7},</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>100</v>
-      </c>
-      <c r="B12">
-        <v>0.24</v>
-      </c>
-      <c r="C12">
-        <v>0.25</v>
-      </c>
-      <c r="E12" t="str">
-        <f t="shared" si="0"/>
-        <v>{100,0.24,0.25},</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>110</v>
-      </c>
-      <c r="B13">
-        <v>-0.54</v>
-      </c>
-      <c r="C13">
-        <v>-0.56999999999999995</v>
-      </c>
-      <c r="E13" t="str">
-        <f t="shared" si="0"/>
-        <v>{110,-0.54,-0.57},</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>120</v>
-      </c>
-      <c r="B14">
-        <v>-0.82</v>
-      </c>
-      <c r="C14">
-        <v>-0.81</v>
-      </c>
-      <c r="E14" t="str">
-        <f t="shared" si="0"/>
-        <v>{120,-0.82,-0.81},</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>130</v>
-      </c>
-      <c r="B15">
-        <v>-1.05</v>
-      </c>
-      <c r="C15">
-        <v>-1.06</v>
-      </c>
-      <c r="E15" t="str">
-        <f t="shared" si="0"/>
-        <v>{130,-1.05,-1.06},</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>140</v>
-      </c>
-      <c r="B16">
-        <v>-1.34</v>
-      </c>
-      <c r="C16">
-        <v>-1.37</v>
-      </c>
-      <c r="E16" t="str">
-        <f t="shared" si="0"/>
-        <v>{140,-1.34,-1.37},</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>150</v>
-      </c>
-      <c r="B17">
-        <v>-1.58</v>
-      </c>
-      <c r="C17">
-        <v>-1.57</v>
-      </c>
-      <c r="E17" t="str">
-        <f t="shared" si="0"/>
-        <v>{150,-1.58,-1.57},</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>160</v>
-      </c>
-      <c r="B18">
-        <v>-1.98</v>
-      </c>
-      <c r="C18">
-        <v>-1.89</v>
-      </c>
-      <c r="E18" t="str">
-        <f t="shared" si="0"/>
-        <v>{160,-1.98,-1.89},</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>170</v>
-      </c>
-      <c r="B19">
-        <v>-2.27</v>
-      </c>
-      <c r="C19">
-        <v>-2.21</v>
-      </c>
-      <c r="E19" t="str">
-        <f t="shared" si="0"/>
-        <v>{170,-2.27,-2.21},</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>180</v>
-      </c>
-      <c r="B20">
-        <v>-2.61</v>
-      </c>
-      <c r="C20" s="1">
-        <v>-2.57</v>
-      </c>
-      <c r="E20" t="str">
-        <f t="shared" si="0"/>
-        <v>{180,-2.61,-2.57},</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>